<commit_message>
removed print statements, added favicons in dashboard base, added config var for event mass mail recepients
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>sahilharpal1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Sahil Harpal</t>
+  </si>
+  <si>
+    <t>CA245368</t>
+  </si>
+  <si>
+    <t>7276801998</t>
+  </si>
+  <si>
+    <t>Indian Institute of Technology Jodhpur</t>
   </si>
 </sst>
 </file>
@@ -415,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,6 +465,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
My Events Page Added
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>garg.10@iitj.ac.in</t>
+  </si>
+  <si>
+    <t>Ayush Shukla</t>
+  </si>
+  <si>
+    <t>CA338219</t>
+  </si>
+  <si>
+    <t>8824879806</t>
+  </si>
+  <si>
+    <t>IIT Bombay</t>
   </si>
 </sst>
 </file>
@@ -415,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,6 +465,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Revert "My Events Page Added"
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,21 +32,6 @@
   </si>
   <si>
     <t>College</t>
-  </si>
-  <si>
-    <t>garg.10@iitj.ac.in</t>
-  </si>
-  <si>
-    <t>Ayush Shukla</t>
-  </si>
-  <si>
-    <t>CA338219</t>
-  </si>
-  <si>
-    <t>8824879806</t>
-  </si>
-  <si>
-    <t>IIT Bombay</t>
   </si>
 </sst>
 </file>
@@ -430,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW3"/>
+  <dimension ref="A1:CW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,23 +450,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Final Home and Schedule
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>sahilharpal1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Sahil Harpal</t>
+  </si>
+  <si>
+    <t>CA245368</t>
+  </si>
+  <si>
+    <t>7276801998</t>
+  </si>
+  <si>
+    <t>Indian Institute of Technology Jodhpur</t>
   </si>
 </sst>
 </file>
@@ -415,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,6 +465,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
fixed broken links and added panelist model
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,18 +32,6 @@
   </si>
   <si>
     <t>College</t>
-  </si>
-  <si>
-    <t>testmail@gmail.com</t>
-  </si>
-  <si>
-    <t>Joel Thomas</t>
-  </si>
-  <si>
-    <t>1346422034</t>
-  </si>
-  <si>
-    <t>IIT Jodhpur</t>
   </si>
 </sst>
 </file>
@@ -427,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW3"/>
+  <dimension ref="A1:CW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,20 +450,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Fixed admin search and Team edit bug
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -34,19 +34,19 @@
     <t>College</t>
   </si>
   <si>
-    <t>garg.10@iitj.ac.in</t>
-  </si>
-  <si>
-    <t>Ayush Shukla</t>
-  </si>
-  <si>
-    <t>CA338219</t>
-  </si>
-  <si>
-    <t>8824879806</t>
-  </si>
-  <si>
-    <t>IIT Bombay</t>
+    <t>sahilharpal1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Sahil Harpal</t>
+  </si>
+  <si>
+    <t>CA245368</t>
+  </si>
+  <si>
+    <t>7276801998</t>
+  </si>
+  <si>
+    <t>Indian Institute of Technology Jodhpur</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Admin Dashboard referred by ... bug
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,6 +32,21 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>sahilharpal1234@gmail.com</t>
+  </si>
+  <si>
+    <t>Sahil Harpal</t>
+  </si>
+  <si>
+    <t>CA245368</t>
+  </si>
+  <si>
+    <t>7276801998</t>
+  </si>
+  <si>
+    <t>Indian Institute of Technology Jodhpur</t>
   </si>
 </sst>
 </file>
@@ -415,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW2"/>
+  <dimension ref="A1:CW3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,6 +465,23 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>

<commit_message>
Added calander icon in event card
</commit_message>
<xml_diff>
--- a/media/workbooks/Campus Ambassador List.xlsx
+++ b/media/workbooks/Campus Ambassador List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Campus Ambassadors</t>
   </si>
@@ -32,21 +32,6 @@
   </si>
   <si>
     <t>College</t>
-  </si>
-  <si>
-    <t>sahilharpal1234@gmail.com</t>
-  </si>
-  <si>
-    <t>Sahil Harpal</t>
-  </si>
-  <si>
-    <t>CA245368</t>
-  </si>
-  <si>
-    <t>7276801998</t>
-  </si>
-  <si>
-    <t>Indian Institute of Technology Jodhpur</t>
   </si>
 </sst>
 </file>
@@ -430,7 +415,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CW3"/>
+  <dimension ref="A1:CW2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,23 +450,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>

</xml_diff>